<commit_message>
continue to transform conversion factors into operations based on well define factors and to add unit tests
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57D260F-C753-4AA8-8983-4E33A9A2A9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8AB915-FB08-4228-B48B-E1F28EEE3CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5580065D-5C90-4291-AD4A-D1811BD528FD}">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,6 +619,12 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="2">
+        <v>45511</v>
+      </c>
+      <c r="C2" s="2">
+        <v>45511</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -635,30 +641,66 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4" s="2">
+        <v>45511</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45511</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5" s="2">
+        <v>45511</v>
+      </c>
+      <c r="C5" s="2">
+        <v>45511</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="2">
+        <v>45511</v>
+      </c>
+      <c r="C6" s="2">
+        <v>45511</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7" s="2">
+        <v>45511</v>
+      </c>
+      <c r="C7" s="2">
+        <v>45511</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" s="2">
+        <v>45511</v>
+      </c>
+      <c r="C8" s="2">
+        <v>45511</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>45511</v>
+      </c>
+      <c r="C9" s="2">
+        <v>45511</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -679,22 +721,22 @@
       </c>
       <c r="B11">
         <f>COUNT(B2:B10)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <f>COUNT(C2:C10)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
         <v>64</v>
       </c>
       <c r="E11">
         <f>A11-B11</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <f>A11-C11</f>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -711,6 +753,12 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
+      <c r="B14" s="2">
+        <v>45511</v>
+      </c>
+      <c r="C14" s="2">
+        <v>45511</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -811,6 +859,10 @@
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
+      </c>
+      <c r="P27">
+        <f>273.15*9/5</f>
+        <v>491.66999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -995,22 +1047,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AUse conversion factors for Energy and implement unit test for energy
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8AB915-FB08-4228-B48B-E1F28EEE3CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E8B6BC-DDC8-405E-9F9B-376781138BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5580065D-5C90-4291-AD4A-D1811BD528FD}">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,6 +769,12 @@
       <c r="A16" t="s">
         <v>16</v>
       </c>
+      <c r="B16" s="2">
+        <v>45512</v>
+      </c>
+      <c r="C16" s="2">
+        <v>45512</v>
+      </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1047,22 +1053,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added more unit choices for Elongation Gradient and Electric Tension, change to use factors and added unit tests
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E8B6BC-DDC8-405E-9F9B-376781138BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB4B374-61F9-4918-9A64-8B9D416F4769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5580065D-5C90-4291-AD4A-D1811BD528FD}">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,6 +748,12 @@
       <c r="A13" t="s">
         <v>13</v>
       </c>
+      <c r="B13" s="2">
+        <v>45512</v>
+      </c>
+      <c r="C13" s="2">
+        <v>45512</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -764,6 +770,12 @@
       <c r="A15" t="s">
         <v>15</v>
       </c>
+      <c r="B15" s="2">
+        <v>45512</v>
+      </c>
+      <c r="C15" s="2">
+        <v>45512</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -779,6 +791,12 @@
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45512</v>
+      </c>
+      <c r="C17" s="2">
+        <v>45512</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -1053,22 +1071,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added some unit choices for dynamic viscosity, use factors and added a unit test
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB4B374-61F9-4918-9A64-8B9D416F4769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB471E7-372D-4BC3-8E9E-7C0DA9BFF7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,6 +803,12 @@
       <c r="A18" t="s">
         <v>18</v>
       </c>
+      <c r="B18" s="2">
+        <v>45512</v>
+      </c>
+      <c r="C18" s="2">
+        <v>45512</v>
+      </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -892,6 +898,10 @@
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
+      </c>
+      <c r="P28">
+        <f>100*0.3048*0.3048/(0.45359237*9.80665)</f>
+        <v>2.0885434233150129</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -1071,22 +1081,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
use factors to calculate DensityRateOfChange coefficients and added some more unit choices and unit tests
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB471E7-372D-4BC3-8E9E-7C0DA9BFF7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6B9C0C-2CBB-434A-BA43-F759EBB1C567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5580065D-5C90-4291-AD4A-D1811BD528FD}">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,6 +814,12 @@
       <c r="A19" t="s">
         <v>19</v>
       </c>
+      <c r="B19" s="2">
+        <v>45512</v>
+      </c>
+      <c r="C19" s="2">
+        <v>45512</v>
+      </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1081,22 +1087,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added some unit choices for density as well as using Factors and defining test units
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6B9C0C-2CBB-434A-BA43-F759EBB1C567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6CD901-0141-424E-8472-6C8623E813A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,6 +840,12 @@
       <c r="A21" t="s">
         <v>21</v>
       </c>
+      <c r="B21" s="2">
+        <v>45512</v>
+      </c>
+      <c r="C21" s="2">
+        <v>45512</v>
+      </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -918,6 +924,10 @@
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
+      </c>
+      <c r="P30">
+        <f>0.3048*0.3048*0.3048/0.45359237</f>
+        <v>6.2427960576144616E-2</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -1087,22 +1097,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added some new unit choices to density gradient temperature, utilize Factors and added a unit test
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6CD901-0141-424E-8472-6C8623E813A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CF3816-FB8D-42DA-B117-990DD552F082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5580065D-5C90-4291-AD4A-D1811BD528FD}">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,6 +851,12 @@
       <c r="A22" t="s">
         <v>22</v>
       </c>
+      <c r="B22" s="2">
+        <v>45512</v>
+      </c>
+      <c r="C22" s="2">
+        <v>45512</v>
+      </c>
       <c r="P22">
         <f>365.25*24*3600/12</f>
         <v>2629800</v>
@@ -1097,22 +1103,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added several new unit choices to density gradient depth, use factors and implemented unit tests
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CF3816-FB8D-42DA-B117-990DD552F082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE1665D-3C9C-45F0-8F6C-9969D84B4F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -590,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5580065D-5C90-4291-AD4A-D1811BD528FD}">
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,6 +602,7 @@
     <col min="2" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.5703125" customWidth="1"/>
     <col min="17" max="17" width="13.28515625" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -788,7 +789,7 @@
         <v>45512</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -799,7 +800,7 @@
         <v>45512</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -810,7 +811,7 @@
         <v>45512</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -821,7 +822,7 @@
         <v>45512</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -836,7 +837,7 @@
         <v>2551442.9759999998</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -847,7 +848,7 @@
         <v>45512</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -862,7 +863,7 @@
         <v>2629800</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -871,7 +872,7 @@
         <v>7889400</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -886,7 +887,7 @@
         <v>31557600</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -895,7 +896,7 @@
         <v>31536000</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -904,16 +905,22 @@
         <v>31622400</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
+      </c>
+      <c r="B27" s="2">
+        <v>45513</v>
+      </c>
+      <c r="C27" s="2">
+        <v>45513</v>
       </c>
       <c r="P27">
         <f>273.15*9/5</f>
         <v>491.66999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -922,12 +929,12 @@
         <v>2.0885434233150129</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -936,92 +943,144 @@
         <v>6.2427960576144616E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P32">
+        <f>0.0254*0.0254*0.0254*100*0.3048/0.45359</f>
+        <v>1.1011656137040059E-3</v>
+      </c>
+      <c r="Q32">
+        <f>P32*30/100</f>
+        <v>3.3034968411120179E-4</v>
+      </c>
+      <c r="R32">
+        <f>Q32/30</f>
+        <v>1.1011656137040059E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P34">
+        <f>3*0.3048</f>
+        <v>0.9144000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P35">
+        <f>P34*P34*P34*100*0.3048/0.45359</f>
+        <v>51.375982872974113</v>
+      </c>
+      <c r="Q35">
+        <f>P35*30/100</f>
+        <v>15.412794861892234</v>
+      </c>
+      <c r="R35">
+        <f>Q35/30</f>
+        <v>0.51375982872974113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P36">
+        <f>0.00454609*100*0.3048/0.45359</f>
+        <v>0.30548473996340308</v>
+      </c>
+      <c r="Q36">
+        <f>P36*30/100</f>
+        <v>9.1645421989020925E-2</v>
+      </c>
+      <c r="R36">
+        <f>Q36/30</f>
+        <v>3.054847399634031E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P37">
+        <f>231*0.0254*0.0254*0.0254*100*0.3048/0.45359</f>
+        <v>0.25436925676562533</v>
+      </c>
+      <c r="Q37">
+        <f>P37*30/100</f>
+        <v>7.6310777029687596E-2</v>
+      </c>
+      <c r="R37">
+        <f>Q37/30</f>
+        <v>2.5436925676562533E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1103,22 +1162,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Used factors for Acceleration and added unit tests
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE1665D-3C9C-45F0-8F6C-9969D84B4F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5ADBBB6-3E5E-4923-B496-F3A71B0F3717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,6 +867,12 @@
       <c r="A23" t="s">
         <v>23</v>
       </c>
+      <c r="B23" s="2">
+        <v>45513</v>
+      </c>
+      <c r="C23" s="2">
+        <v>45513</v>
+      </c>
       <c r="P23">
         <f>365.25*24*3600/4</f>
         <v>7889400</v>
@@ -1162,22 +1168,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added extra unit choice, use factors, implement unit tests dor Compressibility
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5ADBBB6-3E5E-4923-B496-F3A71B0F3717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022379D3-0E5A-4C6A-8853-00E474937E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,6 +897,12 @@
       <c r="A25" t="s">
         <v>25</v>
       </c>
+      <c r="B25" s="2">
+        <v>45513</v>
+      </c>
+      <c r="C25" s="2">
+        <v>45513</v>
+      </c>
       <c r="P25">
         <f>365*24*3600</f>
         <v>31536000</v>
@@ -1168,22 +1174,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added new unit choice, implemented unit test and used factors for electrical capacitance
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022379D3-0E5A-4C6A-8853-00E474937E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AACC57-DFEB-4663-97BB-97007D37419E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5580065D-5C90-4291-AD4A-D1811BD528FD}">
   <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,6 +912,12 @@
       <c r="A26" t="s">
         <v>26</v>
       </c>
+      <c r="B26" s="2">
+        <v>45513</v>
+      </c>
+      <c r="C26" s="2">
+        <v>45513</v>
+      </c>
       <c r="P26">
         <f>366 *24*3600</f>
         <v>31622400</v>
@@ -1174,22 +1180,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added new unit choices, unit tests and use factors for AngleVariationGradient
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AACC57-DFEB-4663-97BB-97007D37419E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999F5D6A-C554-4F23-81A6-E9832767855F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,6 +942,12 @@
       <c r="A28" t="s">
         <v>28</v>
       </c>
+      <c r="B28" s="2">
+        <v>45513</v>
+      </c>
+      <c r="C28" s="2">
+        <v>45513</v>
+      </c>
       <c r="P28">
         <f>100*0.3048*0.3048/(0.45359237*9.80665)</f>
         <v>2.0885434233150129</v>
@@ -1180,22 +1186,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit choices, implemented unit tests and use factors for curvature
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999F5D6A-C554-4F23-81A6-E9832767855F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA2EE44-A287-418F-BD5B-B1A7A5C36C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,6 +957,12 @@
       <c r="A29" t="s">
         <v>29</v>
       </c>
+      <c r="B29" s="2">
+        <v>45514</v>
+      </c>
+      <c r="C29" s="2">
+        <v>45514</v>
+      </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1186,22 +1192,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit choices, unit tests and used Factors for Area
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA2EE44-A287-418F-BD5B-B1A7A5C36C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C61511-AB1C-4006-B5FC-3680CEECA0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5580065D-5C90-4291-AD4A-D1811BD528FD}">
   <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,6 +968,12 @@
       <c r="A30" t="s">
         <v>30</v>
       </c>
+      <c r="B30" s="2">
+        <v>45546</v>
+      </c>
+      <c r="C30" s="2">
+        <v>45516</v>
+      </c>
       <c r="P30">
         <f>0.3048*0.3048*0.3048/0.45359237</f>
         <v>6.2427960576144616E-2</v>
@@ -976,6 +982,12 @@
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
+      </c>
+      <c r="B31" s="2">
+        <v>45516</v>
+      </c>
+      <c r="C31" s="2">
+        <v>45516</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -1192,22 +1204,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit test and used Factors for ImageScale
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C61511-AB1C-4006-B5FC-3680CEECA0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABB7C48-0086-48A1-9934-2326BBBE515F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="U32" sqref="U32"/>
+      <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,6 +994,12 @@
       <c r="A32" t="s">
         <v>32</v>
       </c>
+      <c r="B32" s="2">
+        <v>45516</v>
+      </c>
+      <c r="C32" s="2">
+        <v>45516</v>
+      </c>
       <c r="P32">
         <f>0.0254*0.0254*0.0254*100*0.3048/0.45359</f>
         <v>1.1011656137040059E-3</v>
@@ -1204,22 +1210,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modified list of unit choices, added unit tests and used Factors for Pressure
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABB7C48-0086-48A1-9934-2326BBBE515F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B9FC9F-0239-4407-B2BB-6940563EC56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+      <selection activeCell="U39" sqref="U39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,6 +1017,12 @@
       <c r="A33" t="s">
         <v>33</v>
       </c>
+      <c r="B33" s="2">
+        <v>45516</v>
+      </c>
+      <c r="C33" s="2">
+        <v>45516</v>
+      </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1210,22 +1216,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit tests and used factors for Heat Transfer Coefficient
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B9FC9F-0239-4407-B2BB-6940563EC56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2D34D1-C3D4-4BED-9533-84202CA90931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="U39" sqref="U39"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,6 +1028,12 @@
       <c r="A34" t="s">
         <v>34</v>
       </c>
+      <c r="B34" s="2">
+        <v>45516</v>
+      </c>
+      <c r="C34" s="2">
+        <v>45516</v>
+      </c>
       <c r="P34">
         <f>3*0.3048</f>
         <v>0.9144000000000001</v>
@@ -1092,6 +1098,10 @@
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
+      </c>
+      <c r="P39">
+        <f>3600*0.3048*0.3048*5/(9*1054.35)</f>
+        <v>0.17622808365343576</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -1216,22 +1226,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit tests and used Factors for Pressure Loss Constant
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2D34D1-C3D4-4BED-9533-84202CA90931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF856828-D79D-4485-9633-4776FEC1BB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,6 +1043,12 @@
       <c r="A35" t="s">
         <v>35</v>
       </c>
+      <c r="B35" s="2">
+        <v>45516</v>
+      </c>
+      <c r="C35" s="2">
+        <v>45516</v>
+      </c>
       <c r="P35">
         <f>P34*P34*P34*100*0.3048/0.45359</f>
         <v>51.375982872974113</v>
@@ -1108,6 +1114,10 @@
       <c r="A40" t="s">
         <v>40</v>
       </c>
+      <c r="P40">
+        <f>60*60*100000*0.001/(0.001*0.001)</f>
+        <v>360000000000</v>
+      </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1118,16 +1128,28 @@
       <c r="A42" t="s">
         <v>42</v>
       </c>
+      <c r="P42">
+        <f>0.45/(0.0254*0.0254)</f>
+        <v>697.50139500278999</v>
+      </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
+      <c r="P43">
+        <f>393149903724510</f>
+        <v>393149903724510</v>
+      </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
+      <c r="P44">
+        <f>60*60*6896/(100*0.00454609*0.00454609)</f>
+        <v>12012231545.292404</v>
+      </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1143,108 +1165,116 @@
       <c r="A47" t="s">
         <v>47</v>
       </c>
+      <c r="P47">
+        <f>1/0.000145</f>
+        <v>6896.5517241379312</v>
+      </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="P49">
+        <f>0.453592*9.85/(0.0254*0.0254)</f>
+        <v>6925.2297104594209</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63">
         <f>COUNTA(A13:A62)</f>
         <v>50</v>
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
added unit tests and used Factors for Volumetric flowrate
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF856828-D79D-4485-9633-4776FEC1BB37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9F8220-AAF1-4D11-8B75-D686C8DE7572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="S48" sqref="S48"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,6 +1066,12 @@
       <c r="A36" t="s">
         <v>36</v>
       </c>
+      <c r="B36" s="2">
+        <v>45516</v>
+      </c>
+      <c r="C36" s="2">
+        <v>45516</v>
+      </c>
       <c r="P36">
         <f>0.00454609*100*0.3048/0.45359</f>
         <v>0.30548473996340308</v>
@@ -1083,6 +1089,12 @@
       <c r="A37" t="s">
         <v>37</v>
       </c>
+      <c r="B37" s="2">
+        <v>45516</v>
+      </c>
+      <c r="C37" s="2">
+        <v>45516</v>
+      </c>
       <c r="P37">
         <f>231*0.0254*0.0254*0.0254*100*0.3048/0.45359</f>
         <v>0.25436925676562533</v>
@@ -1192,6 +1204,10 @@
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
+      </c>
+      <c r="P51">
+        <f>543455.698925542*365.25</f>
+        <v>198497194.03255421</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -1256,22 +1272,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unt choices, unit tests, used factors for Resistivity
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9F8220-AAF1-4D11-8B75-D686C8DE7572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA4CEFE-B391-4ADA-91B3-4E64119D8F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>Base Quantity</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>remains</t>
+  </si>
+  <si>
+    <t>12.0.2024</t>
   </si>
 </sst>
 </file>
@@ -593,7 +596,7 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,6 +1115,12 @@
       <c r="A38" t="s">
         <v>38</v>
       </c>
+      <c r="B38" s="2">
+        <v>45516</v>
+      </c>
+      <c r="C38" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1272,7 +1281,7 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
@@ -1283,7 +1292,7 @@
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>

</xml_diff>

<commit_message>
added unit choices, unit tests, used Factors for Magnetic Flux
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA4CEFE-B391-4ADA-91B3-4E64119D8F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED49163F-AF1B-44B4-B983-1E516D816C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>Base Quantity</t>
   </si>
@@ -231,9 +231,6 @@
   </si>
   <si>
     <t>remains</t>
-  </si>
-  <si>
-    <t>12.0.2024</t>
   </si>
 </sst>
 </file>
@@ -596,7 +593,7 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,13 +1115,19 @@
       <c r="B38" s="2">
         <v>45516</v>
       </c>
-      <c r="C38" t="s">
-        <v>65</v>
+      <c r="C38" s="2">
+        <v>45516</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
+      </c>
+      <c r="B39" s="2">
+        <v>45516</v>
+      </c>
+      <c r="C39" s="2">
+        <v>45516</v>
       </c>
       <c r="P39">
         <f>3600*0.3048*0.3048*5/(9*1054.35)</f>
@@ -1281,22 +1284,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added unit tests and used factors for volumetric flow rate of change
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED49163F-AF1B-44B4-B983-1E516D816C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA4EC37-B742-4D11-8C52-DA65566C0453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,6 +1138,12 @@
       <c r="A40" t="s">
         <v>40</v>
       </c>
+      <c r="B40" s="2">
+        <v>45516</v>
+      </c>
+      <c r="C40" s="2">
+        <v>45516</v>
+      </c>
       <c r="P40">
         <f>60*60*100000*0.001/(0.001*0.001)</f>
         <v>360000000000</v>
@@ -1284,22 +1290,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit choices, unit tests, and used factors for Frequency Rate of Change
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA4EC37-B742-4D11-8C52-DA65566C0453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6A8760-FF44-4FB5-9E93-648CDA0A8F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -1153,6 +1153,12 @@
       <c r="A41" t="s">
         <v>41</v>
       </c>
+      <c r="B41" s="2">
+        <v>45516</v>
+      </c>
+      <c r="C41" s="2">
+        <v>45516</v>
+      </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1290,22 +1296,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit tests  and used factors for Random walk
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6A8760-FF44-4FB5-9E93-648CDA0A8F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF30656-D5FE-4E01-B5AC-5B7C006776EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="U38" sqref="U38"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,6 +1164,12 @@
       <c r="A42" t="s">
         <v>42</v>
       </c>
+      <c r="B42" s="2">
+        <v>45516</v>
+      </c>
+      <c r="C42" s="2">
+        <v>45516</v>
+      </c>
       <c r="P42">
         <f>0.45/(0.0254*0.0254)</f>
         <v>697.50139500278999</v>
@@ -1296,22 +1302,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit choices, unit tests and used Factors for velovity
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF30656-D5FE-4E01-B5AC-5B7C006776EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC2F675-6F06-43B0-8EEB-FED57292E771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,6 +1179,12 @@
       <c r="A43" t="s">
         <v>43</v>
       </c>
+      <c r="B43" s="2">
+        <v>45516</v>
+      </c>
+      <c r="C43" s="2">
+        <v>45516</v>
+      </c>
       <c r="P43">
         <f>393149903724510</f>
         <v>393149903724510</v>
@@ -1302,22 +1308,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit choices, unit tests and used factors for Interfacial Tension and Force Gradient
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC2F675-6F06-43B0-8EEB-FED57292E771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183CCEE6-848B-4AA2-8CB8-D64FDA0F0E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,6 +1194,12 @@
       <c r="A44" t="s">
         <v>44</v>
       </c>
+      <c r="B44" s="2">
+        <v>45517</v>
+      </c>
+      <c r="C44" s="2">
+        <v>45517</v>
+      </c>
       <c r="P44">
         <f>60*60*6896/(100*0.00454609*0.00454609)</f>
         <v>12012231545.292404</v>
@@ -1202,6 +1208,12 @@
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
+      </c>
+      <c r="B45" s="2">
+        <v>45517</v>
+      </c>
+      <c r="C45" s="2">
+        <v>45517</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
@@ -1308,22 +1320,22 @@
       </c>
       <c r="B63">
         <f>COUNT(B13:B62)</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C63">
         <f>COUNT(C13:C62)</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D63" t="s">
         <v>64</v>
       </c>
       <c r="E63">
         <f>A63-B63</f>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F63">
         <f>A63-C63</f>
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit coices, unit tests and used factors for Volume
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183CCEE6-848B-4AA2-8CB8-D64FDA0F0E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A675DE-745B-471D-80A6-BA5C78BBCB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>Base Quantity</t>
   </si>
@@ -590,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5580065D-5C90-4291-AD4A-D1811BD528FD}">
-  <dimension ref="A1:R65"/>
+  <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,6 +1220,12 @@
       <c r="A46" t="s">
         <v>46</v>
       </c>
+      <c r="B46" s="2">
+        <v>45517</v>
+      </c>
+      <c r="C46" s="2">
+        <v>45517</v>
+      </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -1237,114 +1243,105 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>45</v>
-      </c>
-      <c r="P49">
-        <f>0.453592*9.85/(0.0254*0.0254)</f>
-        <v>6925.2297104594209</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="P50">
+        <f>543455.698925542*365.25</f>
+        <v>198497194.03255421</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
-      </c>
-      <c r="P51">
-        <f>543455.698925542*365.25</f>
-        <v>198497194.03255421</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>61</v>
+      <c r="A62">
+        <f>COUNTA(A13:A61)</f>
+        <v>49</v>
+      </c>
+      <c r="B62">
+        <f>COUNT(B13:B61)</f>
+        <v>34</v>
+      </c>
+      <c r="C62">
+        <f>COUNT(C13:C61)</f>
+        <v>34</v>
+      </c>
+      <c r="D62" t="s">
+        <v>64</v>
+      </c>
+      <c r="E62">
+        <f>A62-B62</f>
+        <v>15</v>
+      </c>
+      <c r="F62">
+        <f>A62-C62</f>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <f>COUNTA(A13:A62)</f>
-        <v>50</v>
-      </c>
-      <c r="B63">
-        <f>COUNT(B13:B62)</f>
-        <v>33</v>
-      </c>
-      <c r="C63">
-        <f>COUNT(C13:C62)</f>
-        <v>33</v>
-      </c>
-      <c r="D63" t="s">
-        <v>64</v>
-      </c>
-      <c r="E63">
-        <f>A63-B63</f>
-        <v>17</v>
-      </c>
-      <c r="F63">
-        <f>A63-C63</f>
-        <v>17</v>
+      <c r="A63" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A64" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added unit choices, unit tests and used Factors for Specific heat capacity
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A675DE-745B-471D-80A6-BA5C78BBCB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212AC380-81EE-4B98-B172-EF87D1D11D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5580065D-5C90-4291-AD4A-D1811BD528FD}">
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,6 +1231,12 @@
       <c r="A47" t="s">
         <v>47</v>
       </c>
+      <c r="B47" s="2">
+        <v>45517</v>
+      </c>
+      <c r="C47" s="2">
+        <v>45517</v>
+      </c>
       <c r="P47">
         <f>1/0.000145</f>
         <v>6896.5517241379312</v>
@@ -1317,22 +1323,22 @@
       </c>
       <c r="B62">
         <f>COUNT(B13:B61)</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C62">
         <f>COUNT(C13:C61)</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
       </c>
       <c r="E62">
         <f>A62-B62</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F62">
         <f>A62-C62</f>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit tests and used factors for Wave Number
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212AC380-81EE-4B98-B172-EF87D1D11D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C357D02-D15B-45E0-B9D2-2484A49F21AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,6 +1246,12 @@
       <c r="A48" t="s">
         <v>48</v>
       </c>
+      <c r="B48" s="2">
+        <v>45517</v>
+      </c>
+      <c r="C48" s="2">
+        <v>45517</v>
+      </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -1323,22 +1329,22 @@
       </c>
       <c r="B62">
         <f>COUNT(B13:B61)</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C62">
         <f>COUNT(C13:C61)</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
       </c>
       <c r="E62">
         <f>A62-B62</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F62">
         <f>A62-C62</f>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit tests and used factors for specific heat capacity temperature gradient
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C357D02-D15B-45E0-B9D2-2484A49F21AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590079C1-D34A-43A8-98B3-12D9CD05D114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,6 +1257,12 @@
       <c r="A49" t="s">
         <v>49</v>
       </c>
+      <c r="B49" s="2">
+        <v>45517</v>
+      </c>
+      <c r="C49" s="2">
+        <v>45517</v>
+      </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -1329,22 +1335,22 @@
       </c>
       <c r="B62">
         <f>COUNT(B13:B61)</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C62">
         <f>COUNT(C13:C61)</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
       </c>
       <c r="E62">
         <f>A62-B62</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F62">
         <f>A62-C62</f>
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit tests and used factors for Material Strength
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590079C1-D34A-43A8-98B3-12D9CD05D114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C9D905-80FB-4154-89E0-5003921BC6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,6 +1268,12 @@
       <c r="A50" t="s">
         <v>50</v>
       </c>
+      <c r="B50" s="2">
+        <v>45517</v>
+      </c>
+      <c r="C50" s="2">
+        <v>45517</v>
+      </c>
       <c r="P50">
         <f>543455.698925542*365.25</f>
         <v>198497194.03255421</v>
@@ -1335,22 +1341,22 @@
       </c>
       <c r="B62">
         <f>COUNT(B13:B61)</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C62">
         <f>COUNT(C13:C61)</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
       </c>
       <c r="E62">
         <f>A62-B62</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F62">
         <f>A62-C62</f>
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit tests and used factors for magnetic flux density
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C9D905-80FB-4154-89E0-5003921BC6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6110741-544A-4364-A2A1-C3A68A7997CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,6 +1283,12 @@
       <c r="A51" t="s">
         <v>51</v>
       </c>
+      <c r="B51" s="2">
+        <v>45517</v>
+      </c>
+      <c r="C51" s="2">
+        <v>45517</v>
+      </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -1341,22 +1347,22 @@
       </c>
       <c r="B62">
         <f>COUNT(B13:B61)</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C62">
         <f>COUNT(C13:C61)</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
       </c>
       <c r="E62">
         <f>A62-B62</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F62">
         <f>A62-C62</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit tests and used factors for temperature gradient
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6110741-544A-4364-A2A1-C3A68A7997CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032AB160-218B-49D6-A346-DC1833B12CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,6 +1294,12 @@
       <c r="A52" t="s">
         <v>52</v>
       </c>
+      <c r="B52" s="2">
+        <v>45517</v>
+      </c>
+      <c r="C52" s="2">
+        <v>45517</v>
+      </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -1347,22 +1353,22 @@
       </c>
       <c r="B62">
         <f>COUNT(B13:B61)</f>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C62">
         <f>COUNT(C13:C61)</f>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
       </c>
       <c r="E62">
         <f>A62-B62</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62">
         <f>A62-C62</f>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit tests and used Factors for Frequency
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032AB160-218B-49D6-A346-DC1833B12CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DAFECE-0581-4F87-8AB6-2CDA7F8EEDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,6 +1305,12 @@
       <c r="A53" t="s">
         <v>53</v>
       </c>
+      <c r="B53" s="2">
+        <v>45517</v>
+      </c>
+      <c r="C53" s="2">
+        <v>45517</v>
+      </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
@@ -1353,22 +1359,22 @@
       </c>
       <c r="B62">
         <f>COUNT(B13:B61)</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C62">
         <f>COUNT(C13:C61)</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
       </c>
       <c r="E62">
         <f>A62-B62</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62">
         <f>A62-C62</f>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit choices, unit tests and used factors for mass rate
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DAFECE-0581-4F87-8AB6-2CDA7F8EEDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3262F7E-F55E-4948-958D-29C02EBD9629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,6 +1316,12 @@
       <c r="A54" t="s">
         <v>54</v>
       </c>
+      <c r="B54" s="2">
+        <v>45517</v>
+      </c>
+      <c r="C54" s="2">
+        <v>45517</v>
+      </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
@@ -1359,22 +1365,22 @@
       </c>
       <c r="B62">
         <f>COUNT(B13:B61)</f>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C62">
         <f>COUNT(C13:C61)</f>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
       </c>
       <c r="E62">
         <f>A62-B62</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62">
         <f>A62-C62</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit tests and used factors for torque gradient
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3262F7E-F55E-4948-958D-29C02EBD9629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA9883A-AD88-4AEC-87BB-29AF0298D7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5580065D-5C90-4291-AD4A-D1811BD528FD}">
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,6 +1327,12 @@
       <c r="A55" t="s">
         <v>55</v>
       </c>
+      <c r="B55" s="2">
+        <v>45517</v>
+      </c>
+      <c r="C55" s="2">
+        <v>45517</v>
+      </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -1365,22 +1371,22 @@
       </c>
       <c r="B62">
         <f>COUNT(B13:B61)</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C62">
         <f>COUNT(C13:C61)</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
       </c>
       <c r="E62">
         <f>A62-B62</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62">
         <f>A62-C62</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit tests and used factors for thermal conductivity
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA9883A-AD88-4AEC-87BB-29AF0298D7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FD6F44-EBA4-40BE-A48B-E6E799F1E6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>Base Quantity</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>remains</t>
+  </si>
+  <si>
+    <t>14.8.22024</t>
   </si>
 </sst>
 </file>
@@ -593,7 +596,7 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,6 +1341,12 @@
       <c r="A56" t="s">
         <v>56</v>
       </c>
+      <c r="B56" s="2">
+        <v>45518</v>
+      </c>
+      <c r="C56" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -1371,7 +1380,7 @@
       </c>
       <c r="B62">
         <f>COUNT(B13:B61)</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C62">
         <f>COUNT(C13:C61)</f>
@@ -1382,7 +1391,7 @@
       </c>
       <c r="E62">
         <f>A62-B62</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F62">
         <f>A62-C62</f>

</xml_diff>

<commit_message>
added unit tests and used factors for Thermal Conductivity temperature gradient
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FD6F44-EBA4-40BE-A48B-E6E799F1E6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C8D71F-E24E-4163-A45A-1340894FC830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>Base Quantity</t>
   </si>
@@ -231,9 +231,6 @@
   </si>
   <si>
     <t>remains</t>
-  </si>
-  <si>
-    <t>14.8.22024</t>
   </si>
 </sst>
 </file>
@@ -595,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5580065D-5C90-4291-AD4A-D1811BD528FD}">
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1344,13 +1341,19 @@
       <c r="B56" s="2">
         <v>45518</v>
       </c>
-      <c r="C56" t="s">
-        <v>65</v>
+      <c r="C56" s="2">
+        <v>45518</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
+      </c>
+      <c r="B57" s="2">
+        <v>45518</v>
+      </c>
+      <c r="C57" s="2">
+        <v>45518</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -1380,22 +1383,22 @@
       </c>
       <c r="B62">
         <f>COUNT(B13:B61)</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C62">
         <f>COUNT(C13:C61)</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
       </c>
       <c r="E62">
         <f>A62-B62</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62">
         <f>A62-C62</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit tests and used factors for Proportion
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C8D71F-E24E-4163-A45A-1340894FC830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493D2F4F-64FC-43BA-815C-67E68F3BFC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
+    <workbookView xWindow="53775" yWindow="3225" windowWidth="21600" windowHeight="15435" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5580065D-5C90-4291-AD4A-D1811BD528FD}">
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,6 +1360,12 @@
       <c r="A58" t="s">
         <v>58</v>
       </c>
+      <c r="B58" s="2">
+        <v>45518</v>
+      </c>
+      <c r="C58" s="2">
+        <v>45518</v>
+      </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -1383,22 +1389,22 @@
       </c>
       <c r="B62">
         <f>COUNT(B13:B61)</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C62">
         <f>COUNT(C13:C61)</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
       </c>
       <c r="E62">
         <f>A62-B62</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62">
         <f>A62-C62</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit tests and used factors for Pressure Gradient
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493D2F4F-64FC-43BA-815C-67E68F3BFC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C58562-9751-4429-BC81-A2335E9B9398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="53775" yWindow="3225" windowWidth="21600" windowHeight="15435" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,6 +1371,12 @@
       <c r="A59" t="s">
         <v>59</v>
       </c>
+      <c r="B59" s="2">
+        <v>45518</v>
+      </c>
+      <c r="C59" s="2">
+        <v>45518</v>
+      </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -1389,22 +1395,22 @@
       </c>
       <c r="B62">
         <f>COUNT(B13:B61)</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C62">
         <f>COUNT(C13:C61)</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
       </c>
       <c r="E62">
         <f>A62-B62</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62">
         <f>A62-C62</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit tests and used Factors for mass gradient
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C58562-9751-4429-BC81-A2335E9B9398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D5EC72-CED7-4C4C-9B59-4DED1A4E95B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="53775" yWindow="3225" windowWidth="21600" windowHeight="15435" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,6 +1382,12 @@
       <c r="A60" t="s">
         <v>60</v>
       </c>
+      <c r="B60" s="2">
+        <v>45518</v>
+      </c>
+      <c r="C60" s="2">
+        <v>45518</v>
+      </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -1395,22 +1401,22 @@
       </c>
       <c r="B62">
         <f>COUNT(B13:B61)</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C62">
         <f>COUNT(C13:C61)</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
       </c>
       <c r="E62">
         <f>A62-B62</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62">
         <f>A62-C62</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added unit tests and used factors for stress
</commit_message>
<xml_diff>
--- a/UnitTestDevelopmentPlan.xlsx
+++ b/UnitTestDevelopmentPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSDC\UnitConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D5EC72-CED7-4C4C-9B59-4DED1A4E95B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE3030D-8A2A-44F8-8292-44C4F733DFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="53775" yWindow="3225" windowWidth="21600" windowHeight="15435" xr2:uid="{B94729D1-81BD-449A-AF55-A83842E0F53F}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,6 +1393,12 @@
       <c r="A61" t="s">
         <v>61</v>
       </c>
+      <c r="B61" s="2">
+        <v>45518</v>
+      </c>
+      <c r="C61" s="2">
+        <v>45518</v>
+      </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62">
@@ -1401,22 +1407,22 @@
       </c>
       <c r="B62">
         <f>COUNT(B13:B61)</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C62">
         <f>COUNT(C13:C61)</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
       </c>
       <c r="E62">
         <f>A62-B62</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F62">
         <f>A62-C62</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>